<commit_message>
added multiple files on 28th sept
</commit_message>
<xml_diff>
--- a/my-files/test.xlsx
+++ b/my-files/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,29 +422,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>World!</t>
-        </is>
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="5">
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>dUMMY data</t>
-        </is>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="I9" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Python</t>
-        </is>
+      <c r="J10" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added multiple files on 29th sept
</commit_message>
<xml_diff>
--- a/my-files/test.xlsx
+++ b/my-files/test.xlsx
@@ -1,34 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="37095" windowHeight="11955" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +49,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,70 +348,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="D4" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="E5" t="n">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="F6" t="n">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
-      <c r="G7" t="n">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="H8" t="n">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" t="n">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
-      <c r="J10" t="n">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>